<commit_message>
Fixed the confusion about attack paths, stop using debug data.
We're back to the "full" "game" now.
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t xml:space="preserve">Melee</t>
   </si>
@@ -122,6 +122,42 @@
   </si>
   <si>
     <t xml:space="preserve">Portal Keeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tome Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fringe Mage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementalist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marksman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zen Archer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juggernaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doom Sniper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pugilist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Brawler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Fist</t>
   </si>
 </sst>
 </file>
@@ -221,15 +257,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,6 +402,75 @@
       </c>
       <c r="U4" s="0" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Borders work if drawn manually around the message box.
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -154,10 +154,10 @@
     <t xml:space="preserve">Street Brawler</t>
   </si>
   <si>
+    <t xml:space="preserve">God Hand</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire Fist</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,6 +460,9 @@
       <c r="J7" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="K7" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="M7" s="0" t="s">
         <v>22</v>
       </c>
@@ -467,9 +470,6 @@
         <v>22</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="V7" s="0" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust how EpiTiles are tinted and how they tint their contents
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t xml:space="preserve">Melee</t>
   </si>
@@ -139,25 +139,52 @@
     <t xml:space="preserve">Marksman</t>
   </si>
   <si>
+    <t xml:space="preserve">Juggler</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zen Archer</t>
   </si>
   <si>
     <t xml:space="preserve">Juggernaut</t>
   </si>
   <si>
-    <t xml:space="preserve">Doom Sniper</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pugilist</t>
   </si>
   <si>
     <t xml:space="preserve">Street Brawler</t>
   </si>
   <si>
+    <t xml:space="preserve">Monk</t>
+  </si>
+  <si>
     <t xml:space="preserve">God Hand</t>
   </si>
   <si>
-    <t xml:space="preserve">Monk</t>
+    <t xml:space="preserve">Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royal Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy Guard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crusader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Templar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distant Doom</t>
   </si>
 </sst>
 </file>
@@ -257,10 +284,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,20 +458,20 @@
       <c r="A6" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="C6" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="P6" s="0" t="s">
         <v>22</v>
@@ -460,17 +487,68 @@
       <c r="J7" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="M7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="0" t="s">
+      <c r="S7" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vegetables now count as Materials, which simplifies some code
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t xml:space="preserve">Melee</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Honorable</t>
   </si>
   <si>
-    <t xml:space="preserve">Tricky</t>
+    <t xml:space="preserve">Stealthy</t>
   </si>
   <si>
     <t xml:space="preserve">Glorious</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Tome Master</t>
   </si>
   <si>
-    <t xml:space="preserve">Fringe Mage</t>
+    <t xml:space="preserve">Dropout Mage</t>
   </si>
   <si>
     <t xml:space="preserve">Elementalist</t>
@@ -184,7 +184,28 @@
     <t xml:space="preserve">Templar</t>
   </si>
   <si>
-    <t xml:space="preserve">Distant Doom</t>
+    <t xml:space="preserve">Sniper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Hunter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pact Archer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duskblade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necromancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warp Weaver</t>
   </si>
 </sst>
 </file>
@@ -284,10 +305,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -547,8 +568,49 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L10" s="0" t="s">
+      <c r="A10" s="0" t="s">
         <v>54</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Electric effects, and Thunder Cherries are on cherry trees now!
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t xml:space="preserve">Melee</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Stealthy</t>
   </si>
   <si>
-    <t xml:space="preserve">Glorious</t>
+    <t xml:space="preserve">Commanding</t>
   </si>
   <si>
     <t xml:space="preserve">Sinister</t>
@@ -160,18 +160,18 @@
     <t xml:space="preserve">God Hand</t>
   </si>
   <si>
-    <t xml:space="preserve">Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royal Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">White Knight</t>
+    <t xml:space="preserve">Dreadnought</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shogun</t>
   </si>
   <si>
     <t xml:space="preserve">Death Knight</t>
   </si>
   <si>
+    <t xml:space="preserve">Mamluk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paladin</t>
   </si>
   <si>
@@ -206,6 +206,30 @@
   </si>
   <si>
     <t xml:space="preserve">Warp Weaver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mentalist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ardent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deadeye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exemplar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battle Savant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erased Spy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atom Lord</t>
   </si>
 </sst>
 </file>
@@ -305,10 +329,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -439,7 +463,7 @@
       <c r="G4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>22</v>
       </c>
       <c r="P4" s="0" t="s">
@@ -531,17 +555,17 @@
       <c r="F8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="K8" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="L8" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="M8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="V8" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,6 +635,52 @@
       </c>
       <c r="T11" s="0" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="V13" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I believe this gets ticks working for Conditions.
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -151,85 +151,85 @@
     <t xml:space="preserve">Pugilist</t>
   </si>
   <si>
+    <t xml:space="preserve">Battle Savant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Street Brawler</t>
   </si>
   <si>
+    <t xml:space="preserve">God Hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dreadnought</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shogun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mamluk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paladin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy Guard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crusader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Templar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sniper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Hunter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pact Archer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duskblade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powderwitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necromancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mentalist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dawnblade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deadeye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exemplar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erased Spy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monk</t>
   </si>
   <si>
-    <t xml:space="preserve">God Hand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dreadnought</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shogun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mamluk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paladin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holy Guard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crusader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Templar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sniper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fusilier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wild Hunter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pact Archer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warlock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duskblade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necromancer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warp Weaver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mentalist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ardent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deadeye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exemplar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battle Savant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erased Spy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atom Lord</t>
+    <t xml:space="preserve">Nucleus</t>
   </si>
 </sst>
 </file>
@@ -332,7 +332,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,20 +526,20 @@
       <c r="A7" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="D7" s="0" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="S7" s="0" t="s">
         <v>45</v>
@@ -621,18 +621,19 @@
       <c r="B11" s="0" t="s">
         <v>59</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="E11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="K11" s="0" t="s">
         <v>61</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="N11" s="1"/>
       <c r="T11" s="0" t="s">
         <v>22</v>
       </c>
@@ -673,10 +674,10 @@
       <c r="J13" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="P13" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="Q13" s="0" t="s">
         <v>68</v>
       </c>
       <c r="V13" s="0" t="s">

</xml_diff>

<commit_message>
Throw in the towel on variable-width fonts.
The fixed-width messages look better, I think.
</commit_message>
<xml_diff>
--- a/etc/Design Docs/Archetypes and Aspects.xlsx
+++ b/etc/Design Docs/Archetypes and Aspects.xlsx
@@ -118,19 +118,19 @@
     <t xml:space="preserve">Afatkuq</t>
   </si>
   <si>
+    <t xml:space="preserve">Druid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nganga</t>
   </si>
   <si>
-    <t xml:space="preserve">Portal Keeper</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wizard</t>
   </si>
   <si>
     <t xml:space="preserve">Tome Master</t>
   </si>
   <si>
-    <t xml:space="preserve">Dropout Mage</t>
+    <t xml:space="preserve">Spellthief</t>
   </si>
   <si>
     <t xml:space="preserve">Elementalist</t>
@@ -332,7 +332,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,17 +463,17 @@
       <c r="G4" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="H4" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="K4" s="0" t="s">
         <v>22</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R4" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,10 +649,10 @@
         <v>64</v>
       </c>
       <c r="E12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="P12" s="0" t="s">
         <v>22</v>

</xml_diff>